<commit_message>
atualiza requirements.txt para o Render
</commit_message>
<xml_diff>
--- a/RTD/RTD-python.xlsx
+++ b/RTD/RTD-python.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Sistema\RTD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2141CA0D-9C99-452B-A93D-99837E8A5586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC997BA-5CEC-4614-991F-A58C1B7CDC6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5790" yWindow="1755" windowWidth="21600" windowHeight="11295" xr2:uid="{9CA6D5CF-C1E5-4753-B8C4-2DFFDEC4C27A}"/>
+    <workbookView xWindow="840" yWindow="2835" windowWidth="21600" windowHeight="11295" xr2:uid="{9CA6D5CF-C1E5-4753-B8C4-2DFFDEC4C27A}"/>
   </bookViews>
   <sheets>
     <sheet name="RTD" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
     <t>negocios</t>
   </si>
   <si>
-    <t>bovak22</t>
+    <t>BOVAK22</t>
   </si>
 </sst>
 </file>
@@ -133,70 +133,70 @@
       <tp>
         <v>0</v>
         <stp/>
-        <stp>bovak22</stp>
+        <stp>BOVAK22</stp>
         <stp>DELTA</stp>
         <tr r="G2" s="1"/>
       </tp>
       <tp>
+        <v>0</v>
+        <stp/>
+        <stp>BOVAK22</stp>
+        <stp>THETA</stp>
+        <tr r="H2" s="1"/>
+      </tp>
+      <tp>
+        <v>3.52</v>
+        <stp/>
+        <stp>BOVAK22</stp>
+        <stp>VEXT</stp>
+        <tr r="J2" s="1"/>
+      </tp>
+      <tp>
+        <v>0</v>
+        <stp/>
+        <stp>BOVAK22</stp>
+        <stp>IMPVT</stp>
+        <tr r="I2" s="1"/>
+      </tp>
+      <tp>
         <v>142</v>
         <stp/>
-        <stp>bovak22</stp>
+        <stp>BOVAK22</stp>
         <stp>PEX</stp>
         <tr r="C2" s="1"/>
       </tp>
       <tp>
         <v>3.52</v>
         <stp/>
-        <stp>bovak22</stp>
+        <stp>BOVAK22</stp>
         <stp>ULT</stp>
         <tr r="B2" s="1"/>
       </tp>
       <tp t="s">
         <v>21/11/2025</v>
         <stp/>
-        <stp>bovak22</stp>
+        <stp>BOVAK22</stp>
         <stp>VEN</stp>
         <tr r="D2" s="1"/>
       </tp>
       <tp>
         <v>0</v>
         <stp/>
-        <stp>bovak22</stp>
-        <stp>THETA</stp>
-        <tr r="H2" s="1"/>
-      </tp>
-      <tp>
-        <v>3.52</v>
-        <stp/>
-        <stp>bovak22</stp>
-        <stp>VEXT</stp>
-        <tr r="J2" s="1"/>
-      </tp>
-      <tp>
-        <v>0</v>
-        <stp/>
-        <stp>bovak22</stp>
-        <stp>IMPVT</stp>
-        <tr r="I2" s="1"/>
-      </tp>
-      <tp>
-        <v>0</v>
-        <stp/>
-        <stp>bovak22</stp>
+        <stp>BOVAK22</stp>
         <stp>OVD</stp>
         <tr r="F2" s="1"/>
       </tp>
       <tp>
         <v>0</v>
         <stp/>
-        <stp>bovak22</stp>
+        <stp>BOVAK22</stp>
         <stp>OCP</stp>
         <tr r="E2" s="1"/>
       </tp>
       <tp>
         <v>3500</v>
         <stp/>
-        <stp>bovak22</stp>
+        <stp>BOVAK22</stp>
         <stp>NEG</stp>
         <tr r="K2" s="1"/>
       </tp>
@@ -525,7 +525,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD18"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>